<commit_message>
get the row value from excel sheet
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chamika\Desktop\selenuim\POM\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C51D2EC-A886-4B28-8BFF-69090BD9F177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A446DA-04FB-46FC-9C5C-A19A2CE9E657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10524" yWindow="0" windowWidth="12516" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>chamika</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>nimal</t>
+  </si>
+  <si>
+    <t>nim123</t>
   </si>
 </sst>
 </file>
@@ -351,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -375,8 +384,16 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1234</v>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>